<commit_message>
sort game.db and cards.db; fix regestration and deleted account; fix xlsx cards;
</commit_message>
<xml_diff>
--- a/services/cards.xlsx
+++ b/services/cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Project\services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B16199D-6D80-468F-A0CE-6B5CE66BABE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28AC793-1278-4644-AC2D-7F8C35470603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="3435" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cards" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>security</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>редкий воробей</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>attack</t>
@@ -750,7 +747,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15"/>
@@ -824,7 +821,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -906,18 +903,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="33" customHeight="1">
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="14.25" customHeight="1">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>34</v>
+      <c r="D6" s="4">
+        <v>0</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1143,10 +1140,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="D14">
         <v>35</v>
@@ -1172,10 +1169,10 @@
         <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1193,7 +1190,7 @@
         <v>800</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1201,10 +1198,10 @@
         <v>3</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1233,7 +1230,7 @@
         <v>30</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -1259,10 +1256,10 @@
         <v>3</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1280,7 +1277,7 @@
         <v>750</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>